<commit_message>
completed doctor(infos), model relations (hasOne, hasMany, ..vv) in sequalize - from v72-v77
</commit_message>
<xml_diff>
--- a/bookingCare/design DB Backend HoiDanIT - Used.xlsx
+++ b/bookingCare/design DB Backend HoiDanIT - Used.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="9288" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="9288"/>
   </bookViews>
   <sheets>
     <sheet name="desgin" sheetId="1" r:id="rId1"/>
@@ -1329,8 +1329,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -44258,7 +44258,7 @@
   </sheetPr>
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
completed Doctor schedule/info v80 - v89
</commit_message>
<xml_diff>
--- a/bookingCare/design DB Backend HoiDanIT - Used.xlsx
+++ b/bookingCare/design DB Backend HoiDanIT - Used.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="9288"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="9288" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="desgin" sheetId="1" r:id="rId1"/>
@@ -1329,8 +1329,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -37591,7 +37591,7 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>